<commit_message>
feat: Implement product management API and frontend components
- Added productController.js to handle CRUD operations for products.
- Created productRoutes.js to define API endpoints for product management.
- Developed productExcelUtils.js for reading and writing product data to an Excel file.
- Implemented PrintPreview component to display invoice details.
- Created ProductForm component for adding and editing products.
- Developed ProductList component to display all products with options to edit and delete.
- Added EditProductPage for editing existing products.
- Created ProductsPage to list all products and handle deletions.
</commit_message>
<xml_diff>
--- a/DummyBackend/data/data.xlsx
+++ b/DummyBackend/data/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,16 +416,16 @@
         <v>mobileNumber</v>
       </c>
       <c r="E1" t="str">
-        <v>items</v>
+        <v>product</v>
       </c>
       <c r="F1" t="str">
-        <v>product</v>
+        <v>quantity</v>
       </c>
       <c r="G1" t="str">
-        <v>quantity</v>
+        <v>originalPrice</v>
       </c>
       <c r="H1" t="str">
-        <v>price</v>
+        <v>offerPrice</v>
       </c>
       <c r="I1" t="str">
         <v>grandPrice</v>
@@ -444,175 +444,299 @@
       </c>
       <c r="N1" t="str">
         <v>deliveryDate</v>
+      </c>
+      <c r="O1" t="str">
+        <v>price</v>
+      </c>
+      <c r="P1" t="str">
+        <v>taxAmount</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>taxRate</v>
+      </c>
+      <c r="R1" t="str">
+        <v>subTotal</v>
+      </c>
+      <c r="S1" t="str">
+        <v>items</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>INV-20250802-001</v>
+        <v>INV-20250816-006</v>
       </c>
       <c r="B2" t="str">
-        <v>2025-08-02</v>
+        <v>2025-08-16</v>
       </c>
       <c r="C2" t="str">
-        <v>Keshav</v>
+        <v>Ram</v>
       </c>
       <c r="D2" t="str">
-        <v>8879456220</v>
+        <v>7894561230</v>
+      </c>
+      <c r="E2" t="str">
+        <v>zeiss dura vision blue protecgt, Sunglass</v>
       </c>
       <c r="F2" t="str">
-        <v>Sunglasses</v>
+        <v>1, 1</v>
       </c>
       <c r="G2" t="str">
-        <v>1</v>
+        <v>3250, 700</v>
       </c>
       <c r="H2" t="str">
-        <v>1500</v>
+        <v>2800, 600</v>
       </c>
       <c r="I2">
-        <v>1650</v>
+        <v>3740</v>
       </c>
       <c r="J2" t="str">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="K2">
-        <v>650</v>
+        <v>1740</v>
       </c>
       <c r="L2" t="str">
-        <v>ldco</v>
+        <v xml:space="preserve">Abc </v>
       </c>
       <c r="M2" t="str">
-        <v>2025-08-02</v>
+        <v>2025-08-16</v>
       </c>
       <c r="N2" t="str">
-        <v>2025-08-04</v>
+        <v>2025-08-17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>INV-20250802-002</v>
+        <v>INV-20250816-005</v>
       </c>
       <c r="B3" t="str">
-        <v>2025-08-02</v>
+        <v>2025-08-16</v>
       </c>
       <c r="C3" t="str">
-        <v>Kunal</v>
+        <v>Amit Kumar</v>
       </c>
       <c r="D3" t="str">
-        <v>7894561230</v>
+        <v>9876589870</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Sunglass, Red Frame</v>
       </c>
       <c r="F3" t="str">
-        <v>Sunglasses</v>
+        <v>2, 2</v>
       </c>
       <c r="G3" t="str">
-        <v>1</v>
+        <v>700, 650</v>
       </c>
       <c r="H3" t="str">
-        <v>1500</v>
+        <v>600, 450</v>
       </c>
       <c r="I3">
-        <v>1650</v>
+        <v>2310</v>
       </c>
       <c r="J3" t="str">
-        <v>1650</v>
-      </c>
-      <c r="K3" t="str">
+        <v>2310</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" t="str">
-        <v>abc</v>
+        <v>Eldeco Udhyaan - 02</v>
       </c>
       <c r="M3" t="str">
-        <v>2025-08-02</v>
+        <v>2025-08-16</v>
       </c>
       <c r="N3" t="str">
-        <v>2025-08-04</v>
+        <v>2025-08-18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>INV-20250802-003</v>
+        <v>INV-20250816-004</v>
       </c>
       <c r="B4" t="str">
-        <v>2025-08-02</v>
+        <v>2025-08-16</v>
       </c>
       <c r="C4" t="str">
-        <v>kunal</v>
+        <v>Kunal</v>
       </c>
       <c r="D4" t="str">
-        <v>7894456123</v>
+        <v>7894561230</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Lens, Frame</v>
       </c>
       <c r="F4" t="str">
-        <v>Frame</v>
+        <v>1, 1</v>
       </c>
       <c r="G4" t="str">
-        <v>1</v>
+        <v>900, 1000</v>
       </c>
       <c r="H4" t="str">
-        <v>1200</v>
+        <v>700, 700</v>
       </c>
       <c r="I4">
-        <v>1320</v>
+        <v>1540</v>
       </c>
       <c r="J4" t="str">
-        <v>1320</v>
-      </c>
-      <c r="K4" t="str">
-        <v/>
+        <v>999</v>
+      </c>
+      <c r="K4">
+        <v>541</v>
       </c>
       <c r="L4" t="str">
-        <v>abc</v>
+        <v>ldco</v>
       </c>
       <c r="M4" t="str">
-        <v>2025-08-02</v>
+        <v>2025-08-16</v>
       </c>
       <c r="N4" t="str">
-        <v/>
+        <v>2025-08-20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>INV-20250804-001</v>
+        <v>INV-20250816-003</v>
       </c>
       <c r="B5" t="str">
-        <v>2025-08-04</v>
+        <v>2025-08-16</v>
       </c>
       <c r="C5" t="str">
-        <v>Ajit</v>
+        <v>Keshav</v>
       </c>
       <c r="D5" t="str">
-        <v>8794525225</v>
+        <v>7894561230</v>
+      </c>
+      <c r="E5" t="str">
+        <v>sunglass</v>
       </c>
       <c r="F5" t="str">
-        <v>Frame, Lens</v>
-      </c>
-      <c r="G5" t="str">
-        <v>1, 1</v>
-      </c>
-      <c r="H5" t="str">
-        <v>1200, 800</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>2200</v>
+        <v>660</v>
       </c>
       <c r="J5" t="str">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="K5">
+        <v>160</v>
+      </c>
+      <c r="L5" t="str">
+        <v>ldco</v>
+      </c>
+      <c r="M5" t="str">
+        <v>2025-08-16</v>
+      </c>
+      <c r="N5" t="str">
+        <v/>
+      </c>
+      <c r="O5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>INV-20250816-002</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2025-08-16</v>
+      </c>
+      <c r="C6" t="str">
+        <v>kUNAL</v>
+      </c>
+      <c r="D6" t="str">
+        <v>7894561230</v>
+      </c>
+      <c r="E6" t="str">
+        <v>sunglass</v>
+      </c>
+      <c r="F6" t="str">
+        <v>1</v>
+      </c>
+      <c r="I6" t="str">
+        <v>805.00</v>
+      </c>
+      <c r="J6" t="str">
+        <v>400</v>
+      </c>
+      <c r="K6" t="str">
+        <v>405.00</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <v>2025-08-16</v>
+      </c>
+      <c r="N6" t="str">
+        <v/>
+      </c>
+      <c r="O6" t="str">
         <v>700</v>
       </c>
-      <c r="L5" t="str">
-        <v>abc</v>
-      </c>
-      <c r="M5" t="str">
-        <v>2025-08-04</v>
-      </c>
-      <c r="N5" t="str">
-        <v>2025-08-05</v>
+      <c r="P6" t="str">
+        <v>105.00</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>15</v>
+      </c>
+      <c r="R6" t="str">
+        <v>700.00</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>INV-20250816-001</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2025-08-16</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Keshav</v>
+      </c>
+      <c r="D7" t="str">
+        <v>7794561230</v>
+      </c>
+      <c r="E7" t="str">
+        <v>sunglass</v>
+      </c>
+      <c r="F7" t="str">
+        <v>1</v>
+      </c>
+      <c r="I7" t="str">
+        <v>770.00</v>
+      </c>
+      <c r="J7" t="str">
+        <v>500</v>
+      </c>
+      <c r="K7" t="str">
+        <v>270.00</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <v>2025-08-16</v>
+      </c>
+      <c r="N7" t="str">
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <v>700</v>
+      </c>
+      <c r="P7" t="str">
+        <v>70.00</v>
+      </c>
+      <c r="Q7" t="str">
+        <v>10</v>
+      </c>
+      <c r="R7" t="str">
+        <v>700.00</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>